<commit_message>
cap nhay " thoat web"
</commit_message>
<xml_diff>
--- a/USDCAD/Data_USDCAD.xlsx
+++ b/USDCAD/Data_USDCAD.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\UiPath\Automatic\Automatic\USDCAD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\UiPath\Automatic\USDCAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FCB025-0271-4F02-8785-02D3920B4D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="3030" windowWidth="14355" windowHeight="12060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="675" yWindow="3030" windowWidth="14355" windowHeight="12060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
   <si>
     <t>Khoi luong</t>
   </si>
@@ -59,7 +58,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -370,7 +369,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -414,30 +413,30 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>189</v>
+        <v>17</v>
       </c>
       <c r="B3">
-        <v>432</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
+        <v>893</v>
+      </c>
+      <c r="C3">
+        <v>2056</v>
       </c>
       <c r="D3">
-        <v>3961</v>
+        <v>12134</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>198.05</v>
+        <v>191</v>
       </c>
       <c r="B4">
-        <v>1015.8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
+        <v>1446.6</v>
+      </c>
+      <c r="C4">
+        <v>5183.6000000000004</v>
       </c>
       <c r="D4">
-        <v>13054.8</v>
+        <v>16791.2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -456,30 +455,30 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>53.19</v>
+        <v>52.36</v>
       </c>
       <c r="B6">
-        <v>53</v>
+        <v>66.02</v>
       </c>
       <c r="C6">
-        <v>47.28</v>
+        <v>71.14</v>
       </c>
       <c r="D6">
-        <v>51.79</v>
+        <v>67.709999999999994</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>52.08</v>
+        <v>61.84</v>
       </c>
       <c r="B7">
-        <v>52.21</v>
+        <v>66.61</v>
       </c>
       <c r="C7">
-        <v>40.54</v>
+        <v>64.42</v>
       </c>
       <c r="D7">
-        <v>61.52</v>
+        <v>59.88</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -513,15 +512,15 @@
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>"Rsi sắp giao : " &amp;E39&amp; "; Rsi đang : " &amp;A6&amp; ";"</f>
-        <v>Rsi sắp giao : 1.11; Rsi đang : 53.19;</v>
+        <v>Rsi sắp giao : -9.48; Rsi đang : 52.36;</v>
       </c>
       <c r="E39">
         <f>A6-A7</f>
-        <v>1.1099999999999994</v>
+        <v>-9.480000000000004</v>
       </c>
       <c r="F39">
         <f>A3-A4</f>
-        <v>-9.0500000000000114</v>
+        <v>-174</v>
       </c>
       <c r="G39">
         <v>200</v>
@@ -530,15 +529,15 @@
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>"Rsi sắp giao : " &amp;E40&amp; "; Rsi đang : " &amp;B6&amp; ";"</f>
-        <v>Rsi sắp giao : 0.789999999999999; Rsi đang : 53;</v>
+        <v>Rsi sắp giao : -0.590000000000003; Rsi đang : 66.02;</v>
       </c>
       <c r="E40">
         <f>B6-B7</f>
-        <v>0.78999999999999915</v>
+        <v>-0.59000000000000341</v>
       </c>
       <c r="F40">
         <f>B3-B4</f>
-        <v>-583.79999999999995</v>
+        <v>-553.59999999999991</v>
       </c>
       <c r="G40">
         <v>2000</v>
@@ -547,21 +546,21 @@
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f>"Rsi sắp giao : " &amp;E41&amp; "; Rsi đang : " &amp;C6&amp; ";"</f>
-        <v>Rsi sắp giao : 6.74; Rsi đang : 47.28;</v>
+        <v>Rsi sắp giao : 6.72; Rsi đang : 71.14;</v>
       </c>
       <c r="E41">
         <f>C6-C7</f>
-        <v>6.740000000000002</v>
+        <v>6.7199999999999989</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f>"Rsi sắp giao : " &amp;E42&amp; "; Rsi đang : " &amp;D6&amp; ";"</f>
-        <v>Rsi sắp giao : -9.73; Rsi đang : 51.79;</v>
+        <v>Rsi sắp giao : 7.82999999999999; Rsi đang : 67.71;</v>
       </c>
       <c r="E42">
         <f>D6-D7</f>
-        <v>-9.730000000000004</v>
+        <v>7.8299999999999912</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cap nhat toi uu
</commit_message>
<xml_diff>
--- a/USDCAD/Data_USDCAD.xlsx
+++ b/USDCAD/Data_USDCAD.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="7">
   <si>
     <t>Khoi luong</t>
   </si>
@@ -370,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -381,9 +381,13 @@
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.140625" customWidth="1"/>
     <col min="3" max="4" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -396,8 +400,20 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -410,36 +426,72 @@
       <c r="D2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="B3">
-        <v>893</v>
+        <v>441</v>
       </c>
       <c r="C3">
-        <v>2056</v>
+        <v>441</v>
       </c>
       <c r="D3">
-        <v>12134</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4921</v>
+      </c>
+      <c r="F3">
+        <v>371</v>
+      </c>
+      <c r="G3">
+        <v>857</v>
+      </c>
+      <c r="H3">
+        <v>857</v>
+      </c>
+      <c r="I3">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>191</v>
+        <v>403.65</v>
       </c>
       <c r="B4">
-        <v>1446.6</v>
+        <v>1965.6</v>
       </c>
       <c r="C4">
-        <v>5183.6000000000004</v>
+        <v>4068</v>
       </c>
       <c r="D4">
-        <v>16791.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16907.599999999999</v>
+      </c>
+      <c r="F4">
+        <v>472.85</v>
+      </c>
+      <c r="G4">
+        <v>1926.35</v>
+      </c>
+      <c r="H4">
+        <v>4554.8</v>
+      </c>
+      <c r="I4">
+        <v>16735.849999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -452,36 +504,72 @@
       <c r="D5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>52.36</v>
+        <v>51.52</v>
       </c>
       <c r="B6">
-        <v>66.02</v>
+        <v>59.21</v>
       </c>
       <c r="C6">
-        <v>71.14</v>
+        <v>65.010000000000005</v>
       </c>
       <c r="D6">
-        <v>67.709999999999994</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>66.849999999999994</v>
+      </c>
+      <c r="F6">
+        <v>55.72</v>
+      </c>
+      <c r="G6">
+        <v>63.39</v>
+      </c>
+      <c r="H6">
+        <v>69.52</v>
+      </c>
+      <c r="I6">
+        <v>67.97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>61.84</v>
+        <v>49.16</v>
       </c>
       <c r="B7">
-        <v>66.61</v>
+        <v>63.32</v>
       </c>
       <c r="C7">
-        <v>64.42</v>
+        <v>68.22</v>
       </c>
       <c r="D7">
-        <v>59.88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>62.17</v>
+      </c>
+      <c r="F7">
+        <v>62.17</v>
+      </c>
+      <c r="G7">
+        <v>64.87</v>
+      </c>
+      <c r="H7">
+        <v>68.7</v>
+      </c>
+      <c r="I7">
+        <v>62.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -494,8 +582,20 @@
       <c r="D8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -506,61 +606,83 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>"Rsi sắp giao : " &amp;E39&amp; "; Rsi đang : " &amp;A6&amp; ";"</f>
-        <v>Rsi sắp giao : -9.48; Rsi đang : 52.36;</v>
+        <v>Rsi sắp giao : 2.36000000000001; Rsi đang : 51.52;</v>
       </c>
       <c r="E39">
         <f>A6-A7</f>
-        <v>-9.480000000000004</v>
+        <v>2.3600000000000065</v>
       </c>
       <c r="F39">
         <f>A3-A4</f>
-        <v>-174</v>
+        <v>-325.64999999999998</v>
       </c>
       <c r="G39">
-        <v>200</v>
+        <f>A4-F4</f>
+        <v>-69.200000000000045</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>"Rsi sắp giao : " &amp;E40&amp; "; Rsi đang : " &amp;B6&amp; ";"</f>
-        <v>Rsi sắp giao : -0.590000000000003; Rsi đang : 66.02;</v>
+        <v>Rsi sắp giao : -4.11; Rsi đang : 59.21;</v>
       </c>
       <c r="E40">
         <f>B6-B7</f>
-        <v>-0.59000000000000341</v>
+        <v>-4.1099999999999994</v>
       </c>
       <c r="F40">
         <f>B3-B4</f>
-        <v>-553.59999999999991</v>
+        <v>-1524.6</v>
       </c>
       <c r="G40">
-        <v>2000</v>
+        <f>B4-G4</f>
+        <v>39.25</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f>"Rsi sắp giao : " &amp;E41&amp; "; Rsi đang : " &amp;C6&amp; ";"</f>
-        <v>Rsi sắp giao : 6.72; Rsi đang : 71.14;</v>
+        <v>Rsi sắp giao : -3.20999999999999; Rsi đang : 65.01;</v>
       </c>
       <c r="E41">
         <f>C6-C7</f>
-        <v>6.7199999999999989</v>
+        <v>-3.2099999999999937</v>
+      </c>
+      <c r="G41">
+        <f>C4-H4</f>
+        <v>-486.80000000000018</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f>"Rsi sắp giao : " &amp;E42&amp; "; Rsi đang : " &amp;D6&amp; ";"</f>
-        <v>Rsi sắp giao : 7.82999999999999; Rsi đang : 67.71;</v>
+        <v>Rsi sắp giao : 4.67999999999999; Rsi đang : 66.85;</v>
       </c>
       <c r="E42">
         <f>D6-D7</f>
-        <v>7.8299999999999912</v>
+        <v>4.6799999999999926</v>
+      </c>
+      <c r="G42">
+        <f>D4-I4</f>
+        <v>171.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>